<commit_message>
date wise expense added
</commit_message>
<xml_diff>
--- a/PersonalExpenseTracking/PersonalExpenseTracking.xlsx
+++ b/PersonalExpenseTracking/PersonalExpenseTracking.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8ded4e9b9b367109/DataAnalytics/Excel_Projects/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8ded4e9b9b367109/DataAnalytics/Excel_Projects/PersonalExpenseTracking/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="422" documentId="8_{77BC2D35-FD7A-2948-BD76-F98EC76E3B7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C2A0DB92-8085-C94A-B9E3-EA3FCC33ABC4}"/>
+  <xr:revisionPtr revIDLastSave="470" documentId="8_{77BC2D35-FD7A-2948-BD76-F98EC76E3B7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{78F293C9-BA93-1D48-A7D6-2F76FE0B0160}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{167C66B2-4433-E64B-8FA4-8994A1354F32}"/>
+    <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="19880" xr2:uid="{167C66B2-4433-E64B-8FA4-8994A1354F32}"/>
   </bookViews>
   <sheets>
     <sheet name="PersonalExpenses" sheetId="1" r:id="rId1"/>
@@ -18,9 +18,12 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">PersonalExpenses!$A$3:$D$14</definedName>
+    <definedName name="_xlchart.v2.0" hidden="1">PersonalExpenses!$M$4:$M$6</definedName>
+    <definedName name="_xlchart.v2.1" hidden="1">PersonalExpenses!$N$3</definedName>
+    <definedName name="_xlchart.v2.2" hidden="1">PersonalExpenses!$N$4:$N$6</definedName>
     <definedName name="Slicer_Category">#N/A</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr/>
@@ -48,8 +51,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="36">
   <si>
     <t>Date</t>
   </si>
@@ -155,14 +180,17 @@
   <si>
     <t>Q2</t>
   </si>
+  <si>
+    <t>Date Wise Expense</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="166" formatCode="&quot;₹&quot;#,##0.00"/>
-    <numFmt numFmtId="169" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="&quot;₹&quot;#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -180,7 +208,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -211,8 +239,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor theme="7" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -295,18 +329,128 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="7" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="7" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="7" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="7" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="7" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="7" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="17" fontId="0" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -317,63 +461,26 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="17" fontId="0" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment shrinkToFit="1"/>
+    <xf numFmtId="16" fontId="0" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" shrinkToFit="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" shrinkToFit="1"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1" shrinkToFit="1"/>
+    <xf numFmtId="16" fontId="0" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -390,46 +497,6 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -457,7 +524,31 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode="&quot;₹&quot;#,##0.00"/>
+      <border outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;₹&quot;#,##0.00"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -482,6 +573,15 @@
           <color indexed="64"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1485,6 +1585,320 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-IN" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Date Wise Expense</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-IN" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>PersonalExpenses!$N$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total Amount</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>PersonalExpenses!$M$4:$M$6</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>45413</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45414</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45415</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>PersonalExpenses!$N$4:$N$6</c:f>
+              <c:numCache>
+                <c:formatCode>"₹"#,##0.00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>21619</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>970</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>250</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7E3A-E549-B34B-D27E2FA72EB2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1504808192"/>
+        <c:axId val="1504824080"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="1504808192"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1504824080"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="1504824080"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="&quot;₹&quot;#,##0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1504808192"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1605,6 +2019,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -3114,6 +3568,522 @@
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -3192,8 +4162,8 @@
       <xdr:rowOff>33866</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>25400</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1049867</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>50799</xdr:rowOff>
     </xdr:to>
@@ -3228,8 +4198,8 @@
       <xdr:rowOff>194734</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>25401</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1049867</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>160866</xdr:rowOff>
     </xdr:to>
@@ -3267,10 +4237,10 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>812799</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>211667</xdr:rowOff>
+      <xdr:rowOff>194733</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+      <mc:Choice Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="11" name="Category">
@@ -3293,7 +4263,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -3334,7 +4304,47 @@
     </mc:AlternateContent>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>8467</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>8466</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>8466</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>169332</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7CE183EE-89EF-5D7A-AA1D-A48FDE4FBAC8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/slicerCaches/slicerCache1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3354,14 +4364,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7892F49D-BFBD-FA48-8B79-089B5F04C0BF}" name="Table1" displayName="Table1" ref="A3:E14" totalsRowShown="0" headerRowDxfId="7" tableBorderDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7892F49D-BFBD-FA48-8B79-089B5F04C0BF}" name="Table1" displayName="Table1" ref="A3:E14" totalsRowShown="0" headerRowDxfId="12" tableBorderDxfId="11">
   <autoFilter ref="A3:E14" xr:uid="{7892F49D-BFBD-FA48-8B79-089B5F04C0BF}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{AD4EE414-BFD9-E04B-AD6C-36FD33198D99}" name="Date" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{BD21E9B3-DC39-3940-AB10-465226641206}" name="Category" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{3F59333B-4CEC-D546-9035-0AE56E928A60}" name="Item" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{3371152C-4CB4-E249-B893-E8014AF0D45C}" name="Amount" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{4E9DEE44-0AF5-AC48-A7CD-6A6A4BC26854}" name="Is Major Expense">
+    <tableColumn id="1" xr3:uid="{AD4EE414-BFD9-E04B-AD6C-36FD33198D99}" name="Date" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{BD21E9B3-DC39-3940-AB10-465226641206}" name="Category" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{3F59333B-4CEC-D546-9035-0AE56E928A60}" name="Item" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{3371152C-4CB4-E249-B893-E8014AF0D45C}" name="Amount" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{4E9DEE44-0AF5-AC48-A7CD-6A6A4BC26854}" name="Is Major Expense" dataDxfId="6">
       <calculatedColumnFormula>IF(D4&gt;$D$16,"YES","NO")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3370,10 +4380,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{02AC156F-A909-A64D-AF66-484531E85D2A}" name="Table2" displayName="Table2" ref="K3:L6" totalsRowShown="0" headerRowDxfId="4" tableBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{02AC156F-A909-A64D-AF66-484531E85D2A}" name="Table2" displayName="Table2" ref="K3:L6" totalsRowShown="0" headerRowDxfId="3" tableBorderDxfId="2">
   <autoFilter ref="K3:L6" xr:uid="{02AC156F-A909-A64D-AF66-484531E85D2A}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{76CE59DA-227B-7F48-B8DE-6A43C5BEA10D}" name="Category" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{76CE59DA-227B-7F48-B8DE-6A43C5BEA10D}" name="Category" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{3460107A-7194-2249-8143-FF37D28B6C6D}" name="Total Amount">
       <calculatedColumnFormula>SUMIF($B$4:$B$14,K4,$D$4:$D$14)</calculatedColumnFormula>
     </tableColumn>
@@ -3383,7 +4393,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4ABADB8D-EA6B-2B4D-86B1-165100602D1C}" name="Table3" displayName="Table3" ref="H3:I6" totalsRowShown="0" headerRowDxfId="2" tableBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4ABADB8D-EA6B-2B4D-86B1-165100602D1C}" name="Table3" displayName="Table3" ref="H3:I6" totalsRowShown="0" headerRowDxfId="5" tableBorderDxfId="4">
   <autoFilter ref="H3:I6" xr:uid="{4ABADB8D-EA6B-2B4D-86B1-165100602D1C}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{A751B5F2-EC02-1241-95A7-1ADD82B6234C}" name="Item"/>
@@ -3690,10 +4700,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EA404F4-FFC4-1D4B-9BAE-EAA270CE6445}">
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3701,341 +4711,374 @@
     <col min="1" max="2" width="10.83203125" style="1"/>
     <col min="3" max="3" width="14" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.83203125" style="2"/>
-    <col min="5" max="5" width="16.5" customWidth="1"/>
-    <col min="6" max="6" width="16.5" style="11" customWidth="1"/>
+    <col min="5" max="5" width="16.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5" customWidth="1"/>
     <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="2.33203125" customWidth="1"/>
     <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.83203125" customWidth="1"/>
+    <col min="13" max="13" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="52.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+    <row r="1" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="5"/>
-      <c r="H2" s="9" t="s">
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="26"/>
+      <c r="H2" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="10"/>
-      <c r="K2" s="3" t="s">
+      <c r="I2" s="23"/>
+      <c r="K2" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="L2" s="5"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="N2" s="26"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="21" t="s">
+      <c r="H3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="21" t="s">
+      <c r="I3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="3" t="s">
         <v>24</v>
       </c>
+      <c r="M3" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="N3" s="33" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" s="6">
         <v>45413</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="2">
         <v>15000</v>
       </c>
-      <c r="E4" s="11" t="str">
+      <c r="E4" s="1" t="str">
         <f>IF(D4&gt;$D$16,"YES","NO")</f>
         <v>YES</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="H4" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="22">
+      <c r="I4" s="10">
         <v>30000</v>
       </c>
-      <c r="K4" s="7" t="s">
+      <c r="K4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L4" s="11">
+      <c r="L4">
         <f>SUMIF($B$4:$B$14,K4,$D$4:$D$14)</f>
         <v>15000</v>
       </c>
+      <c r="M4" s="28" cm="1">
+        <f t="array" ref="M4:M6">_xlfn.UNIQUE(Table1[Date])</f>
+        <v>45413</v>
+      </c>
+      <c r="N4" s="30">
+        <f>SUMIF(Table1[Date],M4,Table1[Amount])</f>
+        <v>21619</v>
+      </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="6">
         <v>45413</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="2">
         <v>5000</v>
       </c>
-      <c r="E5" s="11" t="str">
+      <c r="E5" s="1" t="str">
         <f t="shared" ref="E5:E14" si="0">IF(D5&gt;$D$16,"YES","NO")</f>
         <v>YES</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="H5" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="22">
+      <c r="I5" s="10">
         <v>10000</v>
       </c>
-      <c r="K5" s="7" t="s">
+      <c r="K5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L5" s="11">
+      <c r="L5">
         <f>SUMIF($B$4:$B$14,K5,$D$4:$D$14)</f>
         <v>6890</v>
       </c>
+      <c r="M5" s="28">
+        <v>45414</v>
+      </c>
+      <c r="N5" s="30">
+        <f>SUMIF(Table1[Date],M5,Table1[Amount])</f>
+        <v>970</v>
+      </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="14">
+    <row r="6" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
         <v>45413</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="2">
         <v>750</v>
       </c>
-      <c r="E6" s="11" t="str">
+      <c r="E6" s="1" t="str">
         <f t="shared" si="0"/>
         <v>NO</v>
       </c>
-      <c r="H6" s="23" t="s">
+      <c r="H6" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="I6" s="24">
+      <c r="I6" s="12">
         <f>SUM(I4:I5)</f>
         <v>40000</v>
       </c>
-      <c r="K6" s="7" t="s">
+      <c r="K6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="L6" s="11">
+      <c r="L6">
         <f t="shared" ref="L6" si="1">SUMIF($B$4:$B$14,K6,$D$4:$D$14)</f>
         <v>949</v>
       </c>
+      <c r="M6" s="31">
+        <v>45415</v>
+      </c>
+      <c r="N6" s="32">
+        <f>SUMIF(Table1[Date],M6,Table1[Amount])</f>
+        <v>250</v>
+      </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="6">
         <v>45413</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="2">
         <v>500</v>
       </c>
-      <c r="E7" s="11" t="str">
+      <c r="E7" s="1" t="str">
         <f t="shared" si="0"/>
         <v>NO</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" s="6">
         <v>45414</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="2">
         <v>450</v>
       </c>
-      <c r="E8" s="11" t="str">
+      <c r="E8" s="1" t="str">
         <f t="shared" si="0"/>
         <v>NO</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="6">
         <v>45415</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="2">
         <v>250</v>
       </c>
-      <c r="E9" s="11" t="str">
+      <c r="E9" s="1" t="str">
         <f t="shared" si="0"/>
         <v>NO</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" s="6">
         <v>45413</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="2">
         <v>249</v>
       </c>
-      <c r="E10" s="11" t="str">
+      <c r="E10" s="1" t="str">
         <f t="shared" si="0"/>
         <v>NO</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="6">
         <v>45414</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="2">
         <v>200</v>
       </c>
-      <c r="E11" s="11" t="str">
+      <c r="E11" s="1" t="str">
         <f t="shared" si="0"/>
         <v>NO</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" s="14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" s="6">
         <v>45414</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D12" s="2">
         <v>200</v>
       </c>
-      <c r="E12" s="11" t="str">
+      <c r="E12" s="1" t="str">
         <f t="shared" si="0"/>
         <v>NO</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" s="6">
         <v>45413</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="2">
         <v>120</v>
       </c>
-      <c r="E13" s="11" t="str">
+      <c r="E13" s="1" t="str">
         <f t="shared" si="0"/>
         <v>NO</v>
       </c>
-      <c r="H13" s="11"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" s="14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" s="6">
         <v>45414</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="15">
+      <c r="D14" s="2">
         <v>120</v>
       </c>
-      <c r="E14" s="11" t="str">
+      <c r="E14" s="1" t="str">
         <f t="shared" si="0"/>
         <v>NO</v>
       </c>
-      <c r="H14" s="11"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="12" t="s">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="16">
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="7">
         <f>SUM(D4:D14)</f>
         <v>22839</v>
       </c>
-      <c r="E15" s="19"/>
-      <c r="H15" s="11"/>
+      <c r="E15" s="18"/>
     </row>
-    <row r="16" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="18" t="s">
+    <row r="16" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="17">
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="8">
         <f>AVERAGE(D4:D14)</f>
         <v>2076.2727272727275</v>
       </c>
-      <c r="E16" s="20"/>
+      <c r="E16" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="M2:N2"/>
     <mergeCell ref="A15:C15"/>
     <mergeCell ref="A16:C16"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="K2:L2"/>
   </mergeCells>
-  <conditionalFormatting sqref="E4:F14 F1:F1048576">
+  <conditionalFormatting sqref="F1:F1048576 E4:F14">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="YES">
       <formula>NOT(ISERROR(SEARCH("YES",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
   <tableParts count="3">
     <tablePart r:id="rId2"/>
@@ -4062,198 +5105,196 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28" style="31" customWidth="1"/>
+    <col min="1" max="1" width="28" style="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="29"/>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25" t="s">
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="29"/>
-      <c r="B2" s="26">
+      <c r="B2" s="13">
         <v>44927</v>
       </c>
-      <c r="C2" s="26">
+      <c r="C2" s="13">
         <v>44958</v>
       </c>
-      <c r="D2" s="26">
+      <c r="D2" s="13">
         <v>44986</v>
       </c>
-      <c r="E2" s="26">
+      <c r="E2" s="13">
         <v>45017</v>
       </c>
-      <c r="F2" s="26">
+      <c r="F2" s="13">
         <v>45047</v>
       </c>
-      <c r="G2" s="26">
+      <c r="G2" s="13">
         <v>45078</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="4">
         <v>100</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="4">
         <v>85</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="4">
         <v>87</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="4">
         <v>73</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="4">
         <v>68</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="4">
         <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="4">
         <v>42</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="4">
         <v>37</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="4">
         <v>38</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="4">
         <v>32</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="4">
         <v>18</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="4">
         <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="4">
         <v>12</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="4">
         <v>1</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="4">
         <v>4</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="4">
         <v>5</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="4">
         <v>8</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="4">
         <v>17</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="4">
         <v>15</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="4">
         <v>7</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="4">
         <v>12</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="4">
         <v>10</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="4">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="4">
         <v>29</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="4">
         <v>32</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="4">
         <v>38</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="4">
         <v>24</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="4">
         <v>32</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="4">
         <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="30"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
+      <c r="A8" s="17"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
     </row>
     <row r="9" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="27">
+      <c r="B9" s="14">
         <f>B7/B3</f>
         <v>0.28999999999999998</v>
       </c>
-      <c r="C9" s="27">
+      <c r="C9" s="14">
         <f>C7/C3</f>
         <v>0.37647058823529411</v>
       </c>
-      <c r="D9" s="27">
-        <f t="shared" ref="C9:G9" si="0">D7/D3</f>
+      <c r="D9" s="14">
+        <f t="shared" ref="D9:F9" si="0">D7/D3</f>
         <v>0.43678160919540232</v>
       </c>
-      <c r="E9" s="27">
+      <c r="E9" s="14">
         <f t="shared" si="0"/>
         <v>0.32876712328767121</v>
       </c>
-      <c r="F9" s="27">
+      <c r="F9" s="14">
         <f t="shared" si="0"/>
         <v>0.47058823529411764</v>
       </c>
-      <c r="G9" s="27">
+      <c r="G9" s="14">
         <f>G7/G3</f>
         <v>0.29411764705882354</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C15" s="28"/>
+      <c r="C15" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>